<commit_message>
EPBDS-12164 Add more tests
</commit_message>
<xml_diff>
--- a/STUDIO/org.openl.rules.test/test-resources/functionality/EPBDS-12164_SpreadsheetResults_equals_hashCode.xlsx
+++ b/STUDIO/org.openl.rules.test/test-resources/functionality/EPBDS-12164_SpreadsheetResults_equals_hashCode.xlsx
@@ -1,23 +1,24 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="24430"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10111"/>
   <workbookPr defaultThemeVersion="166925"/>
-  <mc:AlternateContent>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\work\Bugz\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/ekosolapova/work/openl-tablets/STUDIO/org.openl.rules.test/test-resources/functionality/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{D94294D7-CC82-4F34-8543-CF1FB9BB6600}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{080F99F7-C3F2-224A-9940-2079631D3027}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10420" xr2:uid="{15E80AD5-A47F-42FB-AE45-2AD76FC9EBD4}"/>
+    <workbookView xWindow="-38400" yWindow="-7080" windowWidth="38400" windowHeight="22340" xr2:uid="{15E80AD5-A47F-42FB-AE45-2AD76FC9EBD4}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
+    <sheet name="Sheet2" sheetId="2" r:id="rId2"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
-    <ext uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
+    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
     </ext>
     <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
@@ -34,7 +35,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="48" uniqueCount="28">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="252" uniqueCount="106">
   <si>
     <t>Spreadsheet SpreadsheetResult mySpr(int a)</t>
   </si>
@@ -63,15 +64,6 @@
     <t>=mySpr(a)</t>
   </si>
   <si>
-    <t>=$mySpr[(a) transform to unique a]</t>
-  </si>
-  <si>
-    <t>=$Step1[(a) transform to unique a]</t>
-  </si>
-  <si>
-    <t>=$Step1[(p) transform to unique p]</t>
-  </si>
-  <si>
     <t>=$Step1[(p) transform unique to p]</t>
   </si>
   <si>
@@ -84,33 +76,18 @@
     <t>A</t>
   </si>
   <si>
-    <t>_res_</t>
-  </si>
-  <si>
     <t>Result</t>
   </si>
   <si>
     <t>1, 1, 1</t>
   </si>
   <si>
-    <t>0.0</t>
-  </si>
-  <si>
     <t>beforeTransformation</t>
   </si>
   <si>
-    <t>$Step1.length()</t>
-  </si>
-  <si>
-    <t>=$Step1.length()</t>
-  </si>
-  <si>
     <t>=length($Step1)</t>
   </si>
   <si>
-    <t>aftreTransformation</t>
-  </si>
-  <si>
     <t>=length($Step2)</t>
   </si>
   <si>
@@ -118,17 +95,274 @@
   </si>
   <si>
     <t>_res_.$afterTransformation</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Spreadsheet SpreadsheetResult spr1(Integer a) </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Spreadsheet SpreadsheetResult spr2(Integer a) </t>
+  </si>
+  <si>
+    <t>Result1</t>
+  </si>
+  <si>
+    <t>Resul2</t>
+  </si>
+  <si>
+    <t>=a+3</t>
+  </si>
+  <si>
+    <t>=a+4</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Spreadsheet SpreadsheetResult spr3(Integer a) </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Spreadsheet SpreadsheetResult spr4(Integer a, Integer b) </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Spreadsheet SpreadsheetResult spr5(Integer a) </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Spreadsheet SpreadsheetResult spr6(Integer a) </t>
+  </si>
+  <si>
+    <t>SteP2</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Spreadsheet SpreadsheetResult spr7(Integer a) </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Spreadsheet SpreadsheetResult spr8(Integer a) </t>
+  </si>
+  <si>
+    <t>=a*2</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Spreadsheet SpreadsheetResult spr9(Integer a) </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Spreadsheet SpreadsheetResult spr10(Integer a) </t>
+  </si>
+  <si>
+    <t>Step2:Float</t>
+  </si>
+  <si>
+    <t>Resul2:Double</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Spreadsheet SpreadsheetResult spr11(Integer a) </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Spreadsheet SpreadsheetResult spr12(Integer a) </t>
+  </si>
+  <si>
+    <t>=spr1(a)</t>
+  </si>
+  <si>
+    <t>=spr2(a)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Spreadsheet SpreadsheetResult spr13(Integer a) </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Spreadsheet SpreadsheetResult spr14(Integer a) </t>
+  </si>
+  <si>
+    <t>=spr7(a)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Spreadsheet SpreadsheetResult spr15(Integer a) </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Spreadsheet SpreadsheetResult spr16(Integer a) </t>
+  </si>
+  <si>
+    <t>=null</t>
+  </si>
+  <si>
+    <t>Spreadsheet SpreadsheetResult result(Integer a)</t>
+  </si>
+  <si>
+    <t>Equal</t>
+  </si>
+  <si>
+    <t>NonEqual</t>
+  </si>
+  <si>
+    <t>Compare1</t>
+  </si>
+  <si>
+    <t>=spr1(a)==spr2(a)</t>
+  </si>
+  <si>
+    <t>=spr1(a)&lt;&gt;spr2(a)</t>
+  </si>
+  <si>
+    <t>//Different orders of column</t>
+  </si>
+  <si>
+    <t>Compare2</t>
+  </si>
+  <si>
+    <t>=spr3(a)==spr4(a, a)</t>
+  </si>
+  <si>
+    <t>=spr3(a)&lt;&gt;spr4(a, a)</t>
+  </si>
+  <si>
+    <t>//Different number of input parameters</t>
+  </si>
+  <si>
+    <t>Compare3</t>
+  </si>
+  <si>
+    <t>=spr5(a)==spr6(a)</t>
+  </si>
+  <si>
+    <t>=spr5(a)&lt;&gt;spr6(a)</t>
+  </si>
+  <si>
+    <t>//Case sensitivity</t>
+  </si>
+  <si>
+    <t>Compare4</t>
+  </si>
+  <si>
+    <t>=spr1(a)==spr2(a+1)</t>
+  </si>
+  <si>
+    <t>=spr1(a)&lt;&gt;spr2(a+1)</t>
+  </si>
+  <si>
+    <t>//Different values</t>
+  </si>
+  <si>
+    <t>Compare5</t>
+  </si>
+  <si>
+    <t>=spr7(a)==spr8(a)</t>
+  </si>
+  <si>
+    <t>=spr7(a)&lt;&gt;spr8(a)</t>
+  </si>
+  <si>
+    <t>//Different Formula, but the smae values</t>
+  </si>
+  <si>
+    <t>Compare6</t>
+  </si>
+  <si>
+    <t>=spr9(a)==spr10(a)</t>
+  </si>
+  <si>
+    <t>=spr9(a)&lt;&gt;spr10(a)</t>
+  </si>
+  <si>
+    <t>//Cast to different types</t>
+  </si>
+  <si>
+    <t>Compare7</t>
+  </si>
+  <si>
+    <t>=spr11(a)==spr12(a)</t>
+  </si>
+  <si>
+    <t>=spr11(a)&lt;&gt;spr12(a)</t>
+  </si>
+  <si>
+    <t>// Different SPR are called</t>
+  </si>
+  <si>
+    <t>Compare8</t>
+  </si>
+  <si>
+    <t>=spr13(a)==spr14(a)</t>
+  </si>
+  <si>
+    <t>=spr13(a)&lt;&gt;spr14(a)</t>
+  </si>
+  <si>
+    <t>// Different SPR are callde</t>
+  </si>
+  <si>
+    <t>Compare9</t>
+  </si>
+  <si>
+    <t>=spr15(a)==spr16(a)</t>
+  </si>
+  <si>
+    <t>=spr15(a)&lt;&gt;spr16(a)</t>
+  </si>
+  <si>
+    <t>// Null comparison</t>
+  </si>
+  <si>
+    <t>Test result resultTest</t>
+  </si>
+  <si>
+    <t>_res_.$Equal$Compare1</t>
+  </si>
+  <si>
+    <t>_res_.$NonEqual$Compare1</t>
+  </si>
+  <si>
+    <t>_res_.$Equal$Compare2</t>
+  </si>
+  <si>
+    <t>_res_.$NonEqual$Compare2</t>
+  </si>
+  <si>
+    <t>_res_.$Equal$Compare3</t>
+  </si>
+  <si>
+    <t>_res_.$NonEqual$Compare3</t>
+  </si>
+  <si>
+    <t>_res_.$Equal$Compare4</t>
+  </si>
+  <si>
+    <t>_res_.$NonEqual$Compare4</t>
+  </si>
+  <si>
+    <t>_res_.$Equal$Compare5</t>
+  </si>
+  <si>
+    <t>_res_.$NonEqual$Compare5</t>
+  </si>
+  <si>
+    <t>_res_.$Equal$Compare6</t>
+  </si>
+  <si>
+    <t>_res_.$NonEqual$Compare6</t>
+  </si>
+  <si>
+    <t>_res_.$Equal$Compare7</t>
+  </si>
+  <si>
+    <t>_res_.$NonEqual$Compare7</t>
+  </si>
+  <si>
+    <t>_res_.$Equal$Compare8</t>
+  </si>
+  <si>
+    <t>_res_.$NonEqual$Compare8</t>
+  </si>
+  <si>
+    <t>_res_.$Equal$Compare9</t>
+  </si>
+  <si>
+    <t>_res_.$NonEqual$Compare9</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <numFmts count="0"/>
   <fonts count="1" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
-      <color theme="1" rgb="000000"/>
+      <color theme="1"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
@@ -142,7 +376,7 @@
       <patternFill patternType="gray125"/>
     </fill>
   </fills>
-  <borders count="5">
+  <borders count="2">
     <border>
       <left/>
       <right/>
@@ -151,32 +385,33 @@
       <diagonal/>
     </border>
     <border>
-      <bottom style="thin"/>
-    </border>
-    <border>
-      <top style="thin"/>
-      <bottom style="thin"/>
-    </border>
-    <border>
-      <left style="thin"/>
-      <top style="thin"/>
-      <bottom style="thin"/>
-    </border>
-    <border>
-      <left style="thin"/>
-      <right style="thin"/>
-      <top style="thin"/>
-      <bottom style="thin"/>
+      <left style="thin">
+        <color auto="1"/>
+      </left>
+      <right style="thin">
+        <color auto="1"/>
+      </right>
+      <top style="thin">
+        <color auto="1"/>
+      </top>
+      <bottom style="thin">
+        <color auto="1"/>
+      </bottom>
+      <diagonal/>
     </border>
   </borders>
   <cellStyleXfs count="1">
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="4">
+  <cellXfs count="6">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" quotePrefix="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="true"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="true"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -497,14 +732,14 @@
       <selection activeCell="E15" sqref="E15"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <sheetData>
-    <row r="4" spans="4:5" x14ac:dyDescent="0.35">
+    <row r="4" spans="2:5" x14ac:dyDescent="0.2">
       <c r="D4" t="s">
         <v>0</v>
       </c>
     </row>
-    <row r="5" spans="4:5" x14ac:dyDescent="0.35">
+    <row r="5" spans="2:5" x14ac:dyDescent="0.2">
       <c r="D5" t="s">
         <v>1</v>
       </c>
@@ -512,7 +747,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="6" spans="4:5" x14ac:dyDescent="0.35">
+    <row r="6" spans="2:5" x14ac:dyDescent="0.2">
       <c r="D6" t="s">
         <v>3</v>
       </c>
@@ -520,7 +755,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="7" spans="4:5" x14ac:dyDescent="0.35">
+    <row r="7" spans="2:5" x14ac:dyDescent="0.2">
       <c r="D7" t="s">
         <v>5</v>
       </c>
@@ -528,84 +763,80 @@
         <v>6</v>
       </c>
     </row>
-    <row r="11" spans="4:5" x14ac:dyDescent="0.35"/>
-    <row r="12" spans="4:5" x14ac:dyDescent="0.35"/>
-    <row r="13" spans="4:5" x14ac:dyDescent="0.35"/>
-    <row r="14" spans="4:5" x14ac:dyDescent="0.35"/>
-    <row r="16">
-      <c r="B16" s="2" t="s">
+    <row r="16" spans="2:5" x14ac:dyDescent="0.2">
+      <c r="B16" s="4" t="s">
+        <v>10</v>
+      </c>
+      <c r="C16" s="4"/>
+    </row>
+    <row r="17" spans="2:3" x14ac:dyDescent="0.2">
+      <c r="B17" s="2" t="s">
+        <v>11</v>
+      </c>
+      <c r="C17" s="2" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="18" spans="2:3" x14ac:dyDescent="0.2">
+      <c r="B18" s="2" t="s">
+        <v>12</v>
+      </c>
+      <c r="C18" s="2" t="s">
         <v>13</v>
       </c>
-      <c r="C16" s="2"/>
-    </row>
-    <row r="17">
-      <c r="B17" t="s" s="2">
+    </row>
+    <row r="19" spans="2:3" x14ac:dyDescent="0.2">
+      <c r="B19" s="2" t="s">
         <v>14</v>
       </c>
-      <c r="C17" s="2" t="s">
-        <v>27</v>
-      </c>
-    </row>
-    <row r="18">
-      <c r="B18" t="s" s="2">
+      <c r="C19" s="2">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="21" spans="2:3" x14ac:dyDescent="0.2">
+      <c r="B21" t="s">
+        <v>7</v>
+      </c>
+      <c r="C21" s="3"/>
+    </row>
+    <row r="22" spans="2:3" x14ac:dyDescent="0.2">
+      <c r="B22" t="s">
+        <v>1</v>
+      </c>
+      <c r="C22" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="23" spans="2:3" x14ac:dyDescent="0.2">
+      <c r="B23" t="s">
+        <v>3</v>
+      </c>
+      <c r="C23" s="1" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="24" spans="2:3" x14ac:dyDescent="0.2">
+      <c r="B24" t="s">
+        <v>5</v>
+      </c>
+      <c r="C24" s="1" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="25" spans="2:3" x14ac:dyDescent="0.2">
+      <c r="B25" t="s">
         <v>15</v>
       </c>
-      <c r="C18" t="s" s="2">
+      <c r="C25" s="1" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="26" spans="2:3" x14ac:dyDescent="0.2">
+      <c r="B26" t="s">
+        <v>18</v>
+      </c>
+      <c r="C26" s="1" t="s">
         <v>17</v>
-      </c>
-    </row>
-    <row r="19">
-      <c r="B19" s="2" t="s">
-        <v>18</v>
-      </c>
-      <c r="C19" s="2" t="n">
-        <v>1.0</v>
-      </c>
-    </row>
-    <row r="21">
-      <c r="B21" t="s" s="0">
-        <v>7</v>
-      </c>
-      <c r="C21" s="3"/>
-    </row>
-    <row r="22">
-      <c r="B22" t="s" s="0">
-        <v>1</v>
-      </c>
-      <c r="C22" t="s" s="0">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="23">
-      <c r="B23" t="s" s="0">
-        <v>3</v>
-      </c>
-      <c r="C23" t="s" s="1">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="24">
-      <c r="B24" t="s" s="0">
-        <v>5</v>
-      </c>
-      <c r="C24" t="s" s="1">
-        <v>12</v>
-      </c>
-    </row>
-    <row r="25">
-      <c r="B25" s="0" t="s">
-        <v>20</v>
-      </c>
-      <c r="C25" s="1" t="s">
-        <v>23</v>
-      </c>
-    </row>
-    <row r="26">
-      <c r="B26" s="0" t="s">
-        <v>26</v>
-      </c>
-      <c r="C26" s="1" t="s">
-        <v>25</v>
       </c>
     </row>
   </sheetData>
@@ -614,4 +845,917 @@
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{3475F19F-EFCE-6A40-A2C8-1012AC16BA3D}">
+  <dimension ref="B2:J79"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection sqref="A1:L81"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
+  <sheetData>
+    <row r="2" spans="2:10" x14ac:dyDescent="0.2">
+      <c r="B2" t="s">
+        <v>20</v>
+      </c>
+      <c r="H2" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="3" spans="2:10" x14ac:dyDescent="0.2">
+      <c r="B3" t="s">
+        <v>1</v>
+      </c>
+      <c r="C3" t="s">
+        <v>22</v>
+      </c>
+      <c r="D3" t="s">
+        <v>23</v>
+      </c>
+      <c r="H3" t="s">
+        <v>1</v>
+      </c>
+      <c r="I3" t="s">
+        <v>23</v>
+      </c>
+      <c r="J3" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="4" spans="2:10" x14ac:dyDescent="0.2">
+      <c r="B4" t="s">
+        <v>3</v>
+      </c>
+      <c r="C4" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="D4" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="H4" t="s">
+        <v>3</v>
+      </c>
+      <c r="I4" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="J4" s="1" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="5" spans="2:10" x14ac:dyDescent="0.2">
+      <c r="B5" t="s">
+        <v>5</v>
+      </c>
+      <c r="C5" s="1" t="s">
+        <v>24</v>
+      </c>
+      <c r="D5" s="1" t="s">
+        <v>25</v>
+      </c>
+      <c r="H5" t="s">
+        <v>5</v>
+      </c>
+      <c r="I5" s="1" t="s">
+        <v>25</v>
+      </c>
+      <c r="J5" s="1" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="8" spans="2:10" x14ac:dyDescent="0.2">
+      <c r="B8" t="s">
+        <v>26</v>
+      </c>
+      <c r="H8" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="9" spans="2:10" x14ac:dyDescent="0.2">
+      <c r="B9" t="s">
+        <v>1</v>
+      </c>
+      <c r="C9" t="s">
+        <v>22</v>
+      </c>
+      <c r="D9" t="s">
+        <v>23</v>
+      </c>
+      <c r="H9" t="s">
+        <v>1</v>
+      </c>
+      <c r="I9" t="s">
+        <v>23</v>
+      </c>
+      <c r="J9" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="10" spans="2:10" x14ac:dyDescent="0.2">
+      <c r="B10" t="s">
+        <v>3</v>
+      </c>
+      <c r="C10" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="D10" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="H10" t="s">
+        <v>3</v>
+      </c>
+      <c r="I10" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="J10" s="1" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="11" spans="2:10" x14ac:dyDescent="0.2">
+      <c r="B11" t="s">
+        <v>5</v>
+      </c>
+      <c r="C11" s="1" t="s">
+        <v>24</v>
+      </c>
+      <c r="D11" s="1" t="s">
+        <v>25</v>
+      </c>
+      <c r="H11" t="s">
+        <v>5</v>
+      </c>
+      <c r="I11" s="1" t="s">
+        <v>25</v>
+      </c>
+      <c r="J11" s="1" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="14" spans="2:10" x14ac:dyDescent="0.2">
+      <c r="B14" t="s">
+        <v>28</v>
+      </c>
+      <c r="H14" t="s">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="15" spans="2:10" x14ac:dyDescent="0.2">
+      <c r="B15" t="s">
+        <v>1</v>
+      </c>
+      <c r="C15" t="s">
+        <v>22</v>
+      </c>
+      <c r="D15" t="s">
+        <v>23</v>
+      </c>
+      <c r="H15" t="s">
+        <v>1</v>
+      </c>
+      <c r="I15" t="s">
+        <v>23</v>
+      </c>
+      <c r="J15" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="16" spans="2:10" x14ac:dyDescent="0.2">
+      <c r="B16" t="s">
+        <v>3</v>
+      </c>
+      <c r="C16" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="D16" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="H16" t="s">
+        <v>3</v>
+      </c>
+      <c r="I16" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="J16" s="1" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="17" spans="2:10" x14ac:dyDescent="0.2">
+      <c r="B17" t="s">
+        <v>5</v>
+      </c>
+      <c r="C17" s="1" t="s">
+        <v>24</v>
+      </c>
+      <c r="D17" s="1" t="s">
+        <v>25</v>
+      </c>
+      <c r="H17" t="s">
+        <v>30</v>
+      </c>
+      <c r="I17" s="1" t="s">
+        <v>25</v>
+      </c>
+      <c r="J17" s="1" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="19" spans="2:10" x14ac:dyDescent="0.2">
+      <c r="B19" t="s">
+        <v>31</v>
+      </c>
+      <c r="H19" t="s">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="20" spans="2:10" x14ac:dyDescent="0.2">
+      <c r="B20" t="s">
+        <v>1</v>
+      </c>
+      <c r="C20" t="s">
+        <v>22</v>
+      </c>
+      <c r="H20" t="s">
+        <v>1</v>
+      </c>
+      <c r="I20" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="21" spans="2:10" x14ac:dyDescent="0.2">
+      <c r="B21" t="s">
+        <v>3</v>
+      </c>
+      <c r="C21" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="H21" t="s">
+        <v>3</v>
+      </c>
+      <c r="I21" s="1" t="s">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="23" spans="2:10" x14ac:dyDescent="0.2">
+      <c r="B23" t="s">
+        <v>34</v>
+      </c>
+      <c r="H23" t="s">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="24" spans="2:10" x14ac:dyDescent="0.2">
+      <c r="B24" t="s">
+        <v>1</v>
+      </c>
+      <c r="C24" t="s">
+        <v>22</v>
+      </c>
+      <c r="D24" t="s">
+        <v>23</v>
+      </c>
+      <c r="H24" t="s">
+        <v>1</v>
+      </c>
+      <c r="I24" t="s">
+        <v>3</v>
+      </c>
+      <c r="J24" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="25" spans="2:10" x14ac:dyDescent="0.2">
+      <c r="B25" t="s">
+        <v>3</v>
+      </c>
+      <c r="C25" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="D25" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="H25" t="s">
+        <v>22</v>
+      </c>
+      <c r="I25" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="J25" s="1" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="26" spans="2:10" x14ac:dyDescent="0.2">
+      <c r="B26" t="s">
+        <v>36</v>
+      </c>
+      <c r="C26" s="1" t="s">
+        <v>24</v>
+      </c>
+      <c r="D26" s="1" t="s">
+        <v>25</v>
+      </c>
+      <c r="H26" t="s">
+        <v>37</v>
+      </c>
+      <c r="I26" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="J26" s="1" t="s">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="30" spans="2:10" x14ac:dyDescent="0.2">
+      <c r="B30" t="s">
+        <v>38</v>
+      </c>
+      <c r="H30" t="s">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="31" spans="2:10" x14ac:dyDescent="0.2">
+      <c r="B31" t="s">
+        <v>1</v>
+      </c>
+      <c r="C31" t="s">
+        <v>22</v>
+      </c>
+      <c r="D31" t="s">
+        <v>23</v>
+      </c>
+      <c r="H31" t="s">
+        <v>1</v>
+      </c>
+      <c r="I31" t="s">
+        <v>22</v>
+      </c>
+      <c r="J31" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="32" spans="2:10" x14ac:dyDescent="0.2">
+      <c r="B32" t="s">
+        <v>3</v>
+      </c>
+      <c r="C32" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="D32" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="H32" t="s">
+        <v>3</v>
+      </c>
+      <c r="I32" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="J32" s="1" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="33" spans="2:10" x14ac:dyDescent="0.2">
+      <c r="B33" t="s">
+        <v>5</v>
+      </c>
+      <c r="C33" s="1" t="s">
+        <v>24</v>
+      </c>
+      <c r="D33" s="1" t="s">
+        <v>40</v>
+      </c>
+      <c r="H33" t="s">
+        <v>5</v>
+      </c>
+      <c r="I33" s="1" t="s">
+        <v>24</v>
+      </c>
+      <c r="J33" s="1" t="s">
+        <v>41</v>
+      </c>
+    </row>
+    <row r="35" spans="2:10" x14ac:dyDescent="0.2">
+      <c r="B35" t="s">
+        <v>42</v>
+      </c>
+      <c r="H35" t="s">
+        <v>43</v>
+      </c>
+    </row>
+    <row r="36" spans="2:10" x14ac:dyDescent="0.2">
+      <c r="B36" t="s">
+        <v>1</v>
+      </c>
+      <c r="C36" t="s">
+        <v>22</v>
+      </c>
+      <c r="D36" t="s">
+        <v>23</v>
+      </c>
+      <c r="H36" t="s">
+        <v>1</v>
+      </c>
+      <c r="I36" t="s">
+        <v>22</v>
+      </c>
+      <c r="J36" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="37" spans="2:10" x14ac:dyDescent="0.2">
+      <c r="B37" t="s">
+        <v>3</v>
+      </c>
+      <c r="C37" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="D37" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="H37" t="s">
+        <v>3</v>
+      </c>
+      <c r="I37" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="J37" s="1" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="38" spans="2:10" x14ac:dyDescent="0.2">
+      <c r="B38" t="s">
+        <v>5</v>
+      </c>
+      <c r="C38" s="1" t="s">
+        <v>24</v>
+      </c>
+      <c r="D38" s="1" t="s">
+        <v>40</v>
+      </c>
+      <c r="H38" t="s">
+        <v>5</v>
+      </c>
+      <c r="I38" s="1" t="s">
+        <v>24</v>
+      </c>
+      <c r="J38" s="1" t="s">
+        <v>44</v>
+      </c>
+    </row>
+    <row r="40" spans="2:10" x14ac:dyDescent="0.2">
+      <c r="B40" t="s">
+        <v>45</v>
+      </c>
+      <c r="H40" t="s">
+        <v>46</v>
+      </c>
+    </row>
+    <row r="41" spans="2:10" x14ac:dyDescent="0.2">
+      <c r="B41" t="s">
+        <v>1</v>
+      </c>
+      <c r="C41" t="s">
+        <v>22</v>
+      </c>
+      <c r="D41" t="s">
+        <v>23</v>
+      </c>
+      <c r="H41" t="s">
+        <v>1</v>
+      </c>
+      <c r="I41" t="s">
+        <v>22</v>
+      </c>
+      <c r="J41" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="42" spans="2:10" x14ac:dyDescent="0.2">
+      <c r="B42" t="s">
+        <v>3</v>
+      </c>
+      <c r="C42" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="D42" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="H42" t="s">
+        <v>3</v>
+      </c>
+      <c r="I42" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="J42" s="1" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="43" spans="2:10" x14ac:dyDescent="0.2">
+      <c r="B43" t="s">
+        <v>5</v>
+      </c>
+      <c r="C43" s="1" t="s">
+        <v>24</v>
+      </c>
+      <c r="D43" s="1" t="s">
+        <v>47</v>
+      </c>
+      <c r="H43" t="s">
+        <v>5</v>
+      </c>
+      <c r="I43" s="1" t="s">
+        <v>24</v>
+      </c>
+      <c r="J43" s="1"/>
+    </row>
+    <row r="47" spans="2:10" x14ac:dyDescent="0.2">
+      <c r="B47" t="s">
+        <v>48</v>
+      </c>
+    </row>
+    <row r="48" spans="2:10" x14ac:dyDescent="0.2">
+      <c r="B48" t="s">
+        <v>1</v>
+      </c>
+      <c r="C48" t="s">
+        <v>49</v>
+      </c>
+      <c r="D48" t="s">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="49" spans="2:8" x14ac:dyDescent="0.2">
+      <c r="B49" t="s">
+        <v>51</v>
+      </c>
+      <c r="C49" s="1" t="s">
+        <v>52</v>
+      </c>
+      <c r="D49" s="1" t="s">
+        <v>53</v>
+      </c>
+      <c r="F49" t="b">
+        <v>1</v>
+      </c>
+      <c r="H49" t="s">
+        <v>54</v>
+      </c>
+    </row>
+    <row r="50" spans="2:8" x14ac:dyDescent="0.2">
+      <c r="B50" t="s">
+        <v>55</v>
+      </c>
+      <c r="C50" s="1" t="s">
+        <v>56</v>
+      </c>
+      <c r="D50" s="1" t="s">
+        <v>57</v>
+      </c>
+      <c r="F50" t="b">
+        <v>1</v>
+      </c>
+      <c r="H50" t="s">
+        <v>58</v>
+      </c>
+    </row>
+    <row r="51" spans="2:8" x14ac:dyDescent="0.2">
+      <c r="B51" t="s">
+        <v>59</v>
+      </c>
+      <c r="C51" s="1" t="s">
+        <v>60</v>
+      </c>
+      <c r="D51" s="1" t="s">
+        <v>61</v>
+      </c>
+      <c r="F51" t="b">
+        <v>0</v>
+      </c>
+      <c r="H51" t="s">
+        <v>62</v>
+      </c>
+    </row>
+    <row r="52" spans="2:8" x14ac:dyDescent="0.2">
+      <c r="B52" t="s">
+        <v>63</v>
+      </c>
+      <c r="C52" s="1" t="s">
+        <v>64</v>
+      </c>
+      <c r="D52" s="1" t="s">
+        <v>65</v>
+      </c>
+      <c r="F52" t="b">
+        <v>0</v>
+      </c>
+      <c r="H52" t="s">
+        <v>66</v>
+      </c>
+    </row>
+    <row r="53" spans="2:8" x14ac:dyDescent="0.2">
+      <c r="B53" t="s">
+        <v>67</v>
+      </c>
+      <c r="C53" s="1" t="s">
+        <v>68</v>
+      </c>
+      <c r="D53" s="1" t="s">
+        <v>69</v>
+      </c>
+      <c r="F53" t="b">
+        <v>1</v>
+      </c>
+      <c r="H53" t="s">
+        <v>70</v>
+      </c>
+    </row>
+    <row r="54" spans="2:8" x14ac:dyDescent="0.2">
+      <c r="B54" t="s">
+        <v>71</v>
+      </c>
+      <c r="C54" s="1" t="s">
+        <v>72</v>
+      </c>
+      <c r="D54" s="1" t="s">
+        <v>73</v>
+      </c>
+      <c r="F54" t="b">
+        <v>0</v>
+      </c>
+      <c r="H54" t="s">
+        <v>74</v>
+      </c>
+    </row>
+    <row r="55" spans="2:8" x14ac:dyDescent="0.2">
+      <c r="B55" t="s">
+        <v>75</v>
+      </c>
+      <c r="C55" s="1" t="s">
+        <v>76</v>
+      </c>
+      <c r="D55" s="1" t="s">
+        <v>77</v>
+      </c>
+      <c r="F55" t="b">
+        <v>1</v>
+      </c>
+      <c r="H55" t="s">
+        <v>78</v>
+      </c>
+    </row>
+    <row r="56" spans="2:8" x14ac:dyDescent="0.2">
+      <c r="B56" t="s">
+        <v>79</v>
+      </c>
+      <c r="C56" s="1" t="s">
+        <v>80</v>
+      </c>
+      <c r="D56" s="1" t="s">
+        <v>81</v>
+      </c>
+      <c r="F56" t="b">
+        <v>0</v>
+      </c>
+      <c r="H56" t="s">
+        <v>82</v>
+      </c>
+    </row>
+    <row r="57" spans="2:8" x14ac:dyDescent="0.2">
+      <c r="B57" t="s">
+        <v>83</v>
+      </c>
+      <c r="C57" s="1" t="s">
+        <v>84</v>
+      </c>
+      <c r="D57" s="1" t="s">
+        <v>85</v>
+      </c>
+      <c r="F57" t="b">
+        <v>1</v>
+      </c>
+      <c r="H57" t="s">
+        <v>86</v>
+      </c>
+    </row>
+    <row r="60" spans="2:8" x14ac:dyDescent="0.2">
+      <c r="B60" s="5" t="s">
+        <v>87</v>
+      </c>
+      <c r="C60" s="5"/>
+      <c r="D60" s="5"/>
+    </row>
+    <row r="61" spans="2:8" x14ac:dyDescent="0.2">
+      <c r="B61" t="s">
+        <v>11</v>
+      </c>
+      <c r="C61" t="s">
+        <v>11</v>
+      </c>
+      <c r="D61">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="62" spans="2:8" x14ac:dyDescent="0.2">
+      <c r="B62" t="s">
+        <v>88</v>
+      </c>
+      <c r="C62" t="s">
+        <v>88</v>
+      </c>
+      <c r="D62" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="63" spans="2:8" x14ac:dyDescent="0.2">
+      <c r="B63" t="s">
+        <v>89</v>
+      </c>
+      <c r="C63" t="s">
+        <v>89</v>
+      </c>
+      <c r="D63" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="64" spans="2:8" x14ac:dyDescent="0.2">
+      <c r="B64" t="s">
+        <v>90</v>
+      </c>
+      <c r="C64" t="s">
+        <v>90</v>
+      </c>
+      <c r="D64" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="65" spans="2:4" x14ac:dyDescent="0.2">
+      <c r="B65" t="s">
+        <v>91</v>
+      </c>
+      <c r="C65" t="s">
+        <v>91</v>
+      </c>
+      <c r="D65" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="66" spans="2:4" x14ac:dyDescent="0.2">
+      <c r="B66" t="s">
+        <v>92</v>
+      </c>
+      <c r="C66" t="s">
+        <v>92</v>
+      </c>
+      <c r="D66" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="67" spans="2:4" x14ac:dyDescent="0.2">
+      <c r="B67" t="s">
+        <v>93</v>
+      </c>
+      <c r="C67" t="s">
+        <v>93</v>
+      </c>
+      <c r="D67" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="68" spans="2:4" x14ac:dyDescent="0.2">
+      <c r="B68" t="s">
+        <v>94</v>
+      </c>
+      <c r="C68" t="s">
+        <v>94</v>
+      </c>
+      <c r="D68" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="69" spans="2:4" x14ac:dyDescent="0.2">
+      <c r="B69" t="s">
+        <v>95</v>
+      </c>
+      <c r="C69" t="s">
+        <v>95</v>
+      </c>
+      <c r="D69" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="70" spans="2:4" x14ac:dyDescent="0.2">
+      <c r="B70" t="s">
+        <v>96</v>
+      </c>
+      <c r="C70" t="s">
+        <v>96</v>
+      </c>
+      <c r="D70" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="71" spans="2:4" x14ac:dyDescent="0.2">
+      <c r="B71" t="s">
+        <v>97</v>
+      </c>
+      <c r="C71" t="s">
+        <v>97</v>
+      </c>
+      <c r="D71" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="72" spans="2:4" x14ac:dyDescent="0.2">
+      <c r="B72" t="s">
+        <v>98</v>
+      </c>
+      <c r="C72" t="s">
+        <v>98</v>
+      </c>
+      <c r="D72" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="73" spans="2:4" x14ac:dyDescent="0.2">
+      <c r="B73" t="s">
+        <v>99</v>
+      </c>
+      <c r="C73" t="s">
+        <v>99</v>
+      </c>
+      <c r="D73" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="74" spans="2:4" x14ac:dyDescent="0.2">
+      <c r="B74" t="s">
+        <v>100</v>
+      </c>
+      <c r="C74" t="s">
+        <v>100</v>
+      </c>
+      <c r="D74" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="75" spans="2:4" x14ac:dyDescent="0.2">
+      <c r="B75" t="s">
+        <v>101</v>
+      </c>
+      <c r="C75" t="s">
+        <v>101</v>
+      </c>
+      <c r="D75" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="76" spans="2:4" x14ac:dyDescent="0.2">
+      <c r="B76" t="s">
+        <v>102</v>
+      </c>
+      <c r="C76" t="s">
+        <v>102</v>
+      </c>
+      <c r="D76" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="77" spans="2:4" x14ac:dyDescent="0.2">
+      <c r="B77" t="s">
+        <v>103</v>
+      </c>
+      <c r="C77" t="s">
+        <v>103</v>
+      </c>
+      <c r="D77" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="78" spans="2:4" x14ac:dyDescent="0.2">
+      <c r="B78" t="s">
+        <v>104</v>
+      </c>
+      <c r="C78" t="s">
+        <v>104</v>
+      </c>
+      <c r="D78" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="79" spans="2:4" x14ac:dyDescent="0.2">
+      <c r="B79" t="s">
+        <v>105</v>
+      </c>
+      <c r="C79" t="s">
+        <v>105</v>
+      </c>
+      <c r="D79" t="b">
+        <v>0</v>
+      </c>
+    </row>
+  </sheetData>
+  <mergeCells count="1">
+    <mergeCell ref="B60:D60"/>
+  </mergeCells>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
 </file>
</xml_diff>